<commit_message>
Author : Bhaskar Mamgai Description : Task Breakdown Sprint 2 File modified : BhaskarMamgai.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/BhaskarMamgai.xlsx
+++ b/TeamDetails/TasksBreakDown/BhaskarMamgai.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhaskar Mamgai\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project\trunk\TeamDetails\TasksBreakDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="45">
   <si>
     <t>Story ID</t>
   </si>
@@ -246,6 +246,33 @@
 3
 4
 5</t>
+  </si>
+  <si>
+    <t>To perform/check clent side validations are as per acceptance criteria.</t>
+  </si>
+  <si>
+    <t>Making a stable bakend re defining bakend databse schema and java files as per reqiured database.</t>
+  </si>
+  <si>
+    <t>To understand how request will be routed to server(routing)</t>
+  </si>
+  <si>
+    <t>T15</t>
+  </si>
+  <si>
+    <t>T16</t>
+  </si>
+  <si>
+    <t>Making a connection with backend database server/jdbc connectivity.</t>
+  </si>
+  <si>
+    <t>T17</t>
+  </si>
+  <si>
+    <t>SVN COMMIT</t>
+  </si>
+  <si>
+    <t>20 min</t>
   </si>
 </sst>
 </file>
@@ -326,7 +353,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -386,11 +413,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -420,32 +467,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -456,22 +479,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -479,20 +544,8 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -794,7 +847,7 @@
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -806,19 +859,19 @@
       <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="28" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="6"/>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -834,12 +887,12 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="11" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="6">
@@ -851,87 +904,87 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="27" t="s">
+    <row r="5" spans="1:7" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="17">
         <v>2</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26">
+      <c r="F5" s="17"/>
+      <c r="G5" s="17">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-    </row>
-    <row r="7" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
+    <row r="6" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9" t="s">
+      <c r="A8" s="18"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="26">
         <v>3</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9">
+      <c r="F8" s="20"/>
+      <c r="G8" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="11"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="16"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="25"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="11"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="12" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="7">
@@ -944,7 +997,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7" t="s">
         <v>15</v>
@@ -962,7 +1015,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7" t="s">
         <v>16</v>
@@ -979,7 +1032,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7" t="s">
         <v>17</v>
@@ -997,7 +1050,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7" t="s">
         <v>18</v>
@@ -1015,7 +1068,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7" t="s">
         <v>19</v>
@@ -1033,7 +1086,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7" t="s">
         <v>20</v>
@@ -1051,7 +1104,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7" t="s">
         <v>22</v>
@@ -1069,7 +1122,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7" t="s">
         <v>24</v>
@@ -1087,7 +1140,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7" t="s">
         <v>29</v>
@@ -1430,6 +1483,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A3:A20"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C10"/>
@@ -1437,11 +1495,6 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="G8:G9"/>
-    <mergeCell ref="A3:A20"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
     <mergeCell ref="F5:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3176,202 +3229,211 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="14" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
     <col min="4" max="4" width="67.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="21" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G1" s="13" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="6">
+        <v>2</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6">
+        <f>E2-F2</f>
+        <v>2</v>
+      </c>
+    </row>
     <row r="3" spans="1:7" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>35</v>
-      </c>
+      <c r="A3" s="22"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>12</v>
+      <c r="C3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="E3" s="6">
         <v>2</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6">
-        <f>E3-F3</f>
+        <f t="shared" ref="G3:G48" si="0">E3-F3</f>
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="6">
+      <c r="A4" s="29"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="17">
         <v>2</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6">
-        <f t="shared" ref="G4:G47" si="0">E4-F4</f>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="26">
-        <v>2</v>
-      </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
+      <c r="A5" s="29"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="20">
+        <v>5</v>
+      </c>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="18">
-        <v>2</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="25" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="11"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+    </row>
+    <row r="9" spans="1:7" s="16" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="35"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="22"/>
     </row>
     <row r="10" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A10" s="22"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="21"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>26</v>
+      <c r="C11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>36</v>
       </c>
       <c r="E11" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="E12" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="E13" s="7">
         <v>3</v>
@@ -3382,153 +3444,164 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E14" s="7">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E15" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E16" s="7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E17" s="7">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="E18" s="7">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E19" s="7">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E20" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="2"/>
+      <c r="C21" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="7">
+        <v>3</v>
+      </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="2"/>
+      <c r="C22" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="F22" s="6"/>
-      <c r="G22" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="G22" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -3831,21 +3904,33 @@
         <v>0</v>
       </c>
     </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="G5:G7"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="A3:A20"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A2:A21"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="G7:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author : Bhaskar Mamgai File modified : BhaskarMamgai.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/BhaskarMamgai.xlsx
+++ b/TeamDetails/TasksBreakDown/BhaskarMamgai.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="46">
   <si>
     <t>Story ID</t>
   </si>
@@ -248,12 +248,6 @@
 5</t>
   </si>
   <si>
-    <t>To perform/check clent side validations are as per acceptance criteria.</t>
-  </si>
-  <si>
-    <t>Making a stable bakend re defining bakend databse schema and java files as per reqiured database.</t>
-  </si>
-  <si>
     <t>To understand how request will be routed to server(routing)</t>
   </si>
   <si>
@@ -266,13 +260,37 @@
     <t>Making a connection with backend database server/jdbc connectivity.</t>
   </si>
   <si>
-    <t>T17</t>
-  </si>
-  <si>
-    <t>SVN COMMIT</t>
-  </si>
-  <si>
-    <t>20 min</t>
+    <r>
+      <t xml:space="preserve">
+*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A user must be provided with login page so that he/she can access their respective pages.
+*When user entered the credential on login page both server side and client side validation should be performed,so that only authentic user logs in web
+app.</t>
+    </r>
+  </si>
+  <si>
+    <t>Understanding "WHY" of the story (Bussiness Rule):</t>
+  </si>
+  <si>
+    <t>Perform/check clent side validations are as per acceptance criteria.</t>
+  </si>
+  <si>
+    <t>Make a stable bakend re-defining bakend database schema and java files as per reqiured database.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> code review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit testing </t>
   </si>
 </sst>
 </file>
@@ -353,7 +371,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -433,11 +451,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -481,8 +530,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -491,6 +540,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -514,28 +578,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -546,6 +595,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -867,7 +928,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="17" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="6"/>
@@ -907,17 +968,17 @@
     <row r="5" spans="1:7" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="20"/>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="25">
         <v>2</v>
       </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17">
+      <c r="F5" s="25"/>
+      <c r="G5" s="25">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -926,7 +987,7 @@
       <c r="A6" s="18"/>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
-      <c r="D6" s="31"/>
+      <c r="D6" s="23"/>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
@@ -935,7 +996,7 @@
       <c r="A7" s="18"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
-      <c r="D7" s="32"/>
+      <c r="D7" s="24"/>
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
@@ -946,10 +1007,10 @@
       <c r="C8" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="31">
         <v>3</v>
       </c>
       <c r="F8" s="20"/>
@@ -959,20 +1020,20 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="21"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="25"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="21"/>
+      <c r="F10" s="26"/>
       <c r="G10" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1483,11 +1544,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A3:A20"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C10"/>
@@ -1496,6 +1552,11 @@
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="F5:F7"/>
+    <mergeCell ref="A3:A20"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3232,7 +3293,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3269,313 +3330,306 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="39"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="42"/>
+    </row>
+    <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="6">
-        <v>2</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6">
-        <f>E2-F2</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>13</v>
+      <c r="C3" s="9"/>
+      <c r="D3" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="E3" s="6">
         <v>2</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6">
-        <f t="shared" ref="G3:G48" si="0">E3-F3</f>
+        <f>E3-F3</f>
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="29" t="s">
+    <row r="4" spans="1:7" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6">
+        <v>2</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6">
+        <f t="shared" ref="G4:G48" si="0">E4-F4</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="21"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D5" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E5" s="25">
         <v>2</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17">
+      <c r="F5" s="25"/>
+      <c r="G5" s="25">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D8" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E8" s="20">
         <v>5</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-    </row>
-    <row r="9" spans="1:7" s="16" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="22"/>
-    </row>
-    <row r="10" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="6" t="s">
+      <c r="F8" s="20"/>
+      <c r="G8" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+    </row>
+    <row r="10" spans="1:7" s="16" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="34"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="27"/>
+    </row>
+    <row r="11" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D11" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="21"/>
-    </row>
-    <row r="11" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6" t="s">
+      <c r="E11" s="26"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="27"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="7">
+      <c r="D12" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="7">
         <v>1</v>
-      </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="7">
-        <v>5</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E13" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E14" s="7">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E15" s="7">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="27"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E16" s="7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E17" s="7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E18" s="7">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="E19" s="7">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E20" s="7">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="E21" s="7">
         <v>3</v>
@@ -3587,21 +3641,21 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="7" t="s">
         <v>44</v>
       </c>
+      <c r="E22" s="7">
+        <v>3</v>
+      </c>
       <c r="F22" s="6"/>
-      <c r="G22" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="G22" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -3917,20 +3971,21 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A2:A21"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="G7:G10"/>
+  <mergeCells count="14">
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="G8:G11"/>
+    <mergeCell ref="A3:A22"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="B8:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author : BhaskarMamgai File modified : BhaskarMamgai.xlsx Description : TasksBreakDown
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/BhaskarMamgai.xlsx
+++ b/TeamDetails/TasksBreakDown/BhaskarMamgai.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
   <si>
     <t>Story ID</t>
   </si>
@@ -251,9 +251,6 @@
     <t>To understand how request will be routed to server(routing)</t>
   </si>
   <si>
-    <t>T15</t>
-  </si>
-  <si>
     <t>T16</t>
   </si>
   <si>
@@ -287,10 +284,67 @@
     <t>Make a stable bakend re-defining bakend database schema and java files as per reqiured database.</t>
   </si>
   <si>
-    <t xml:space="preserve"> code review</t>
-  </si>
-  <si>
     <t xml:space="preserve">Unit testing </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">In backward linkage a database must be defined as per the schema defined and linking a DB to FE so that server side validation is to be done.
+&gt;In forward linking/routing the request so that credentialis is to be validated from backend database(i.e )server. </t>
+    </r>
+  </si>
+  <si>
+    <t>Forward and Backward Linkage:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;Making a block diagram of entire journey of the code so that scope and approach becomes clear.</t>
+    </r>
+  </si>
+  <si>
+    <t>Work Flow and Block Diagram</t>
+  </si>
+  <si>
+    <t>Code review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fetching the req values from database </t>
+  </si>
+  <si>
+    <t>To get app_id,app_status and user_role from value fetched.</t>
+  </si>
+  <si>
+    <t>Getting a response from backend database server</t>
+  </si>
+  <si>
+    <t>T17</t>
+  </si>
+  <si>
+    <t>T18</t>
+  </si>
+  <si>
+    <t>T19</t>
   </si>
 </sst>
 </file>
@@ -371,7 +425,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -482,11 +536,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -530,18 +621,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -554,39 +678,36 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -596,17 +717,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -928,7 +1046,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="31" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="6"/>
@@ -948,7 +1066,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="6"/>
       <c r="C4" s="10" t="s">
         <v>8</v>
@@ -966,81 +1084,81 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="20">
         <v>2</v>
       </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25">
+      <c r="F5" s="20"/>
+      <c r="G5" s="20">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="7" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="29">
         <v>3</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20">
+      <c r="F8" s="23"/>
+      <c r="G8" s="23">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="26"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="24"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="30"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="28"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="26"/>
+      <c r="F10" s="24"/>
       <c r="G10" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7" t="s">
         <v>11</v>
@@ -1058,7 +1176,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7" t="s">
         <v>15</v>
@@ -1076,7 +1194,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7" t="s">
         <v>16</v>
@@ -1093,7 +1211,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7" t="s">
         <v>17</v>
@@ -1111,7 +1229,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7" t="s">
         <v>18</v>
@@ -1129,7 +1247,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7" t="s">
         <v>19</v>
@@ -1147,7 +1265,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7" t="s">
         <v>20</v>
@@ -1165,7 +1283,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7" t="s">
         <v>22</v>
@@ -1183,7 +1301,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7" t="s">
         <v>24</v>
@@ -1201,7 +1319,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7" t="s">
         <v>29</v>
@@ -1544,6 +1662,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A3:A20"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C10"/>
@@ -1552,11 +1675,6 @@
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="F5:F7"/>
-    <mergeCell ref="A3:A20"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3290,10 +3408,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3331,379 +3449,383 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
+      <c r="A2" s="18"/>
       <c r="B2" s="13"/>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="42"/>
+      <c r="D2" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="38"/>
     </row>
     <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="43" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="9"/>
       <c r="D3" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="6">
+        <v>39</v>
+      </c>
+      <c r="E3" s="19">
         <v>2</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6">
+      <c r="F3" s="19"/>
+      <c r="G3" s="19">
         <f>E3-F3</f>
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="44"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="6">
+      <c r="D4" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="51"/>
+    </row>
+    <row r="5" spans="1:7" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="25"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="6">
         <v>2</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6">
-        <f t="shared" ref="G4:G48" si="0">E4-F4</f>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6">
+        <f t="shared" ref="G5:G52" si="0">E5-F5</f>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21" t="s">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="25"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="25">
+      <c r="D6" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="42"/>
+    </row>
+    <row r="7" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="20">
         <v>2</v>
       </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25">
+      <c r="F7" s="20"/>
+      <c r="G7" s="20">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20" t="s">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="32"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D10" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E10" s="23">
         <v>5</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-    </row>
-    <row r="10" spans="1:7" s="16" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="27"/>
-    </row>
-    <row r="11" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="6" t="s">
+      <c r="F10" s="23"/>
+      <c r="G10" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+    </row>
+    <row r="12" spans="1:7" s="16" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="45"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="25"/>
+    </row>
+    <row r="13" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="26"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="26"/>
-    </row>
-    <row r="12" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6" t="s">
+      <c r="E13" s="24"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="24"/>
+    </row>
+    <row r="14" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="25"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="7">
+      <c r="D14" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="7">
         <v>1</v>
-      </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="7">
-        <v>5</v>
-      </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="7">
-        <v>3</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="E15" s="7">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E16" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="E17" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="E18" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F18" s="6"/>
-      <c r="G18" s="6">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
+      <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E19" s="7">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="25"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E20" s="7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="E21" s="7">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E22" s="7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="6"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="2"/>
+      <c r="C23" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="7">
+        <v>6</v>
+      </c>
       <c r="F23" s="6"/>
-      <c r="G23" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="2"/>
+      <c r="C24" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="7">
+        <v>6</v>
+      </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+      <c r="A25" s="25"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="2"/>
+      <c r="C25" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="7">
+        <v>3</v>
+      </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
+      <c r="A26" s="24"/>
       <c r="B26" s="6"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="2"/>
+      <c r="C26" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="7">
+        <v>3</v>
+      </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -3970,22 +4092,72 @@
         <v>0</v>
       </c>
     </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="16">
+    <mergeCell ref="A3:A26"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="D4:G4"/>
     <mergeCell ref="D2:G2"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="G5:G7"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="G8:G11"/>
-    <mergeCell ref="A3:A22"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="D6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author : Bhaskar Mamgai File modified : BhaskarMamgai.xlsx Description : TasksBreakDown
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/BhaskarMamgai.xlsx
+++ b/TeamDetails/TasksBreakDown/BhaskarMamgai.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
   <si>
     <t>Story ID</t>
   </si>
@@ -281,9 +281,6 @@
     <t>Perform/check clent side validations are as per acceptance criteria.</t>
   </si>
   <si>
-    <t>Make a stable bakend re-defining bakend database schema and java files as per reqiured database.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Unit testing </t>
   </si>
   <si>
@@ -345,6 +342,17 @@
   </si>
   <si>
     <t>T19</t>
+  </si>
+  <si>
+    <t>Make a stable bakend re-defining bakend database schema and java files as per reqiured database.
+&gt;Making a database as per the schema defined.
+&gt;Making required java file for backend.</t>
+  </si>
+  <si>
+    <t>T15</t>
+  </si>
+  <si>
+    <t>Make login button functionaL</t>
   </si>
 </sst>
 </file>
@@ -577,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -628,6 +636,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1046,7 +1057,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="32" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="6"/>
@@ -1066,7 +1077,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="6"/>
       <c r="C4" s="10" t="s">
         <v>8</v>
@@ -1084,81 +1095,81 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="32" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="21">
         <v>2</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20">
+      <c r="F5" s="21"/>
+      <c r="G5" s="21">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
     </row>
     <row r="7" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="30">
         <v>3</v>
       </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23">
+      <c r="F8" s="24"/>
+      <c r="G8" s="24">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="24"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="25"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="28"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="29"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="24"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7" t="s">
         <v>11</v>
@@ -1176,7 +1187,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7" t="s">
         <v>15</v>
@@ -1194,7 +1205,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7" t="s">
         <v>16</v>
@@ -1211,7 +1222,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7" t="s">
         <v>17</v>
@@ -1229,7 +1240,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7" t="s">
         <v>18</v>
@@ -1247,7 +1258,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7" t="s">
         <v>19</v>
@@ -1265,7 +1276,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7" t="s">
         <v>20</v>
@@ -1283,7 +1294,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7" t="s">
         <v>22</v>
@@ -1301,7 +1312,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7" t="s">
         <v>24</v>
@@ -1319,7 +1330,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7" t="s">
         <v>29</v>
@@ -3408,10 +3419,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G52"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3454,15 +3468,15 @@
       <c r="C2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
     </row>
     <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="44" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="6"/>
@@ -3480,132 +3494,137 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="6"/>
       <c r="C4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="51"/>
+      <c r="D4" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="52"/>
     </row>
     <row r="5" spans="1:7" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" s="6">
         <v>2</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6">
-        <f t="shared" ref="G5:G52" si="0">E5-F5</f>
+        <f t="shared" ref="G5:G53" si="0">E5-F5</f>
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="17"/>
       <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="42"/>
+      <c r="D6" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="43"/>
     </row>
     <row r="7" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="20">
+      <c r="A7" s="33"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="21">
         <v>2</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20">
+      <c r="F7" s="21"/>
+      <c r="G7" s="21">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23" t="s">
+      <c r="A10" s="26"/>
+      <c r="B10" s="24">
+        <f>SUM(E10:E27)</f>
+        <v>60.5</v>
+      </c>
+      <c r="C10" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="24">
         <v>5</v>
       </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-    </row>
-    <row r="12" spans="1:7" s="16" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="25"/>
-    </row>
-    <row r="13" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" spans="1:7" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="46"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="26"/>
+    </row>
+    <row r="13" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="24"/>
+      <c r="E13" s="20">
+        <v>1.5</v>
+      </c>
       <c r="F13" s="6"/>
-      <c r="G13" s="24"/>
+      <c r="G13" s="25"/>
     </row>
     <row r="14" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="6" t="s">
         <v>15</v>
       </c>
@@ -3620,27 +3639,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7" t="s">
+    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="7">
-        <v>6</v>
+        <v>54</v>
+      </c>
+      <c r="E15" s="6">
+        <v>4</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="7" t="s">
         <v>17</v>
       </c>
@@ -3648,7 +3667,7 @@
         <v>38</v>
       </c>
       <c r="E16" s="7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6">
@@ -3656,13 +3675,13 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="7">
         <v>5</v>
@@ -3674,13 +3693,13 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="6"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E18" s="7">
         <v>4</v>
@@ -3689,8 +3708,8 @@
       <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="7" t="s">
         <v>20</v>
       </c>
@@ -3706,118 +3725,115 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E20" s="7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
-      <c r="B21" s="6"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
       <c r="C21" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="E21" s="7">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="6"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
       <c r="C22" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="7">
+        <v>4</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="E22" s="7">
-        <v>6</v>
-      </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="E23" s="7">
         <v>6</v>
       </c>
       <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
+      <c r="G23" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="6"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
       <c r="C24" s="7" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="E24" s="7">
         <v>6</v>
       </c>
       <c r="F24" s="6"/>
-      <c r="G24" s="6">
-        <f t="shared" si="0"/>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="7">
         <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="7">
-        <v>3</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="24"/>
-      <c r="B26" s="6"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
       <c r="C26" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E26" s="7">
         <v>3</v>
@@ -3829,15 +3845,21 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="2"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="7">
+        <v>3</v>
+      </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -4140,26 +4162,45 @@
         <v>0</v>
       </c>
     </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <f>SUM(E3,E27)</f>
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A3:A26"/>
+    <mergeCell ref="A3:A27"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="D10:D12"/>
-    <mergeCell ref="B10:B13"/>
     <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B10:B27"/>
+    <mergeCell ref="E10:E12"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="G7:G9"/>
     <mergeCell ref="F10:F12"/>
-    <mergeCell ref="E10:E13"/>
     <mergeCell ref="G10:G13"/>
     <mergeCell ref="D6:G6"/>
   </mergeCells>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="83" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Author : Bhaskar Mamgai File modified : BhaskarMamgai.xlsx Description : TasksBreakDown/Sprint 2/Day 1
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/BhaskarMamgai.xlsx
+++ b/TeamDetails/TasksBreakDown/BhaskarMamgai.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
   <si>
     <t>Story ID</t>
   </si>
@@ -347,6 +347,15 @@
   </si>
   <si>
     <t>Code review and Incorporate feedback</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>IN DEV</t>
   </si>
 </sst>
 </file>
@@ -579,7 +588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -635,39 +644,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -686,6 +695,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -734,7 +746,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2908,7 +2920,7 @@
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="54"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="3" t="s">
         <v>52</v>
       </c>
@@ -3481,10 +3493,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3496,9 +3508,10 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3520,22 +3533,25 @@
       <c r="G1" s="13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="13"/>
       <c r="C2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="50"/>
-    </row>
-    <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="51"/>
+    </row>
+    <row r="3" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="6"/>
@@ -3551,21 +3567,24 @@
         <f>E3-F3</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
+      <c r="H3" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="40"/>
       <c r="B4" s="6"/>
       <c r="C4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="47"/>
-    </row>
-    <row r="5" spans="1:7" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="48"/>
+    </row>
+    <row r="5" spans="1:8" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -3580,21 +3599,24 @@
         <f t="shared" ref="G5:G50" si="0">E5-F5</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="32"/>
       <c r="B6" s="17"/>
       <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="53"/>
-    </row>
-    <row r="7" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="54"/>
+    </row>
+    <row r="7" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26"/>
       <c r="B7" s="25"/>
       <c r="C7" s="26"/>
@@ -3609,30 +3631,35 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26"/>
       <c r="B8" s="32"/>
       <c r="C8" s="26"/>
-      <c r="D8" s="42"/>
+      <c r="D8" s="43"/>
       <c r="E8" s="26"/>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="41"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="26"/>
       <c r="B9" s="31"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="42"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="41"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="32"/>
       <c r="B10" s="25">
         <f>SUM(E10:E24)</f>
-        <v>22.5</v>
+        <v>23.5</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>10</v>
@@ -3641,14 +3668,17 @@
         <v>32</v>
       </c>
       <c r="E10" s="25">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F10" s="25"/>
       <c r="G10" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="32"/>
       <c r="B11" s="32"/>
       <c r="C11" s="32"/>
@@ -3656,17 +3686,19 @@
       <c r="E11" s="32"/>
       <c r="F11" s="32"/>
       <c r="G11" s="32"/>
-    </row>
-    <row r="12" spans="1:7" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
+      <c r="H11" s="41"/>
+    </row>
+    <row r="12" spans="1:8" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="41"/>
       <c r="B12" s="32"/>
-      <c r="C12" s="44"/>
+      <c r="C12" s="45"/>
       <c r="D12" s="35"/>
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
       <c r="G12" s="31"/>
-    </row>
-    <row r="13" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="41"/>
+    </row>
+    <row r="13" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="32"/>
       <c r="B13" s="32"/>
       <c r="C13" s="6" t="s">
@@ -3678,12 +3710,14 @@
       <c r="E13" s="20">
         <v>1</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="6">
+        <v>0.5</v>
+      </c>
       <c r="G13" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="32"/>
       <c r="B14" s="32"/>
       <c r="C14" s="6" t="s">
@@ -3692,13 +3726,15 @@
       <c r="D14" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="6">
+        <v>1</v>
+      </c>
       <c r="F14" s="6"/>
       <c r="G14" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="32"/>
       <c r="B15" s="32"/>
       <c r="C15" s="6" t="s">
@@ -3708,15 +3744,17 @@
         <v>47</v>
       </c>
       <c r="E15" s="6">
-        <v>4</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="F15" s="6">
+        <v>2</v>
+      </c>
+      <c r="G15" s="21"/>
+      <c r="H15" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="32"/>
       <c r="B16" s="32"/>
       <c r="C16" s="7" t="s">
@@ -3728,12 +3766,17 @@
       <c r="E16" s="7">
         <v>0.5</v>
       </c>
-      <c r="F16" s="6"/>
+      <c r="F16" s="6">
+        <v>0.5</v>
+      </c>
       <c r="G16" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H16" s="55" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="7" t="s">
@@ -3745,13 +3788,18 @@
       <c r="E17" s="7">
         <v>3</v>
       </c>
-      <c r="F17" s="6"/>
+      <c r="F17" s="6">
+        <v>1</v>
+      </c>
       <c r="G17" s="6">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H17" s="55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="6" t="s">
@@ -3760,16 +3808,21 @@
       <c r="D18" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="7">
-        <v>0</v>
-      </c>
-      <c r="F18" s="6"/>
+      <c r="E18" s="6">
+        <v>4</v>
+      </c>
+      <c r="F18" s="6">
+        <v>2</v>
+      </c>
       <c r="G18" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="32"/>
       <c r="B19" s="32"/>
       <c r="C19" s="7" t="s">
@@ -3779,15 +3832,20 @@
         <v>49</v>
       </c>
       <c r="E19" s="7">
-        <v>0</v>
-      </c>
-      <c r="F19" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0.5</v>
+      </c>
       <c r="G19" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="32"/>
       <c r="B20" s="32"/>
       <c r="C20" s="7" t="s">
@@ -3805,7 +3863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="32"/>
       <c r="B21" s="32"/>
       <c r="C21" s="7" t="s">
@@ -3823,7 +3881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="32"/>
       <c r="B22" s="32"/>
       <c r="C22" s="7" t="s">
@@ -3841,7 +3899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="32"/>
       <c r="B23" s="32"/>
       <c r="C23" s="7" t="s">
@@ -3859,7 +3917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="31"/>
       <c r="B24" s="31"/>
       <c r="C24" s="7" t="s">
@@ -3877,7 +3935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="6"/>
       <c r="C25" s="2"/>
@@ -3889,7 +3947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="6"/>
       <c r="C26" s="2"/>
@@ -3901,7 +3959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="6"/>
       <c r="C27" s="2"/>
@@ -3913,7 +3971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="6"/>
       <c r="C28" s="2"/>
@@ -3925,7 +3983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="6"/>
       <c r="C29" s="2"/>
@@ -3937,7 +3995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="6"/>
       <c r="C30" s="2"/>
@@ -3949,7 +4007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="6"/>
       <c r="C31" s="2"/>
@@ -3961,7 +4019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="6"/>
       <c r="C32" s="2"/>
@@ -4196,7 +4254,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="18">
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="H10:H12"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="F7:F9"/>

</xml_diff>

<commit_message>
Author : Bhaskar Mamgai File modified : BhaskarMamgai.xlsx Description : TasksBreakDown/Sprint 2/Day 2
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/BhaskarMamgai.xlsx
+++ b/TeamDetails/TasksBreakDown/BhaskarMamgai.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="58">
   <si>
     <t>Story ID</t>
   </si>
@@ -275,9 +275,6 @@
     <t>Understanding "WHY" of the story (Bussiness Rule):</t>
   </si>
   <si>
-    <t>Perform/check clent side validations are as per acceptance criteria.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Unit testing </t>
   </si>
   <si>
@@ -357,12 +354,15 @@
   <si>
     <t>IN DEV</t>
   </si>
+  <si>
+    <t>Perform/check client side validations are as per acceptance criteria.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,6 +399,13 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -588,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -647,18 +654,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -671,45 +705,39 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -728,26 +756,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1069,7 +1082,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="34" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="6"/>
@@ -1089,7 +1102,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="6"/>
       <c r="C4" s="10" t="s">
         <v>8</v>
@@ -1107,81 +1120,81 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="23">
         <v>2</v>
       </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30">
+      <c r="F5" s="23"/>
+      <c r="G5" s="23">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
     </row>
     <row r="7" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="32">
         <v>3</v>
       </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25">
+      <c r="F8" s="26"/>
+      <c r="G8" s="26">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="31"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="35"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="31"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="31"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7" t="s">
         <v>11</v>
@@ -1199,7 +1212,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7" t="s">
         <v>15</v>
@@ -1217,7 +1230,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7" t="s">
         <v>16</v>
@@ -1234,7 +1247,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7" t="s">
         <v>17</v>
@@ -1252,7 +1265,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7" t="s">
         <v>18</v>
@@ -1270,7 +1283,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7" t="s">
         <v>19</v>
@@ -1288,7 +1301,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7" t="s">
         <v>20</v>
@@ -1306,7 +1319,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7" t="s">
         <v>22</v>
@@ -1324,7 +1337,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7" t="s">
         <v>24</v>
@@ -1342,7 +1355,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7" t="s">
         <v>29</v>
@@ -1685,6 +1698,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A3:A20"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C10"/>
@@ -1693,11 +1711,6 @@
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="F5:F7"/>
-    <mergeCell ref="A3:A20"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2901,11 +2914,11 @@
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="F3" s="2">
         <v>2</v>
@@ -2920,9 +2933,9 @@
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="38"/>
+      <c r="D4" s="39"/>
       <c r="E4" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
@@ -2937,7 +2950,7 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="37"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="3"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -3493,10 +3506,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10:H12"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3509,9 +3522,10 @@
     <col min="6" max="6" width="11.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3533,25 +3547,25 @@
       <c r="G1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="55" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="13"/>
       <c r="C2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="51"/>
-    </row>
-    <row r="3" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="43"/>
+    </row>
+    <row r="3" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A3" s="48" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="6"/>
@@ -3568,28 +3582,28 @@
         <v>2</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="49"/>
       <c r="B4" s="6"/>
       <c r="C4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="48"/>
-    </row>
-    <row r="5" spans="1:8" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
+      <c r="D4" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="55"/>
+    </row>
+    <row r="5" spans="1:9" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="6">
         <v>2</v>
@@ -3600,107 +3614,107 @@
         <v>2</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
       <c r="B6" s="17"/>
       <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="52" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="54"/>
-    </row>
-    <row r="7" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="27" t="s">
+      <c r="D6" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="47"/>
+    </row>
+    <row r="7" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="35"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="23">
         <v>2</v>
       </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30">
+      <c r="F7" s="23"/>
+      <c r="G7" s="23">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H7" s="41" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="41"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="41"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="25">
+      <c r="H7" s="40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="35"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="40"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="35"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="40"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
+      <c r="B10" s="26">
         <f>SUM(E10:E24)</f>
         <v>23.5</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="25">
-        <v>0</v>
-      </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25">
-        <v>0</v>
-      </c>
-      <c r="H10" s="41" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="41"/>
-    </row>
-    <row r="12" spans="1:8" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="41"/>
-    </row>
-    <row r="13" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="32"/>
+      <c r="E10" s="26">
+        <v>0</v>
+      </c>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26">
+        <v>0</v>
+      </c>
+      <c r="H10" s="40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="40"/>
+    </row>
+    <row r="12" spans="1:9" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="40"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="40"/>
+    </row>
+    <row r="13" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="6" t="s">
         <v>11</v>
       </c>
@@ -3716,32 +3730,41 @@
       <c r="G13" s="21">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="32"/>
+      <c r="H13" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="E14" s="6">
         <v>1</v>
       </c>
-      <c r="F14" s="6"/>
+      <c r="F14" s="6">
+        <v>6</v>
+      </c>
       <c r="G14" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="32"/>
+        <v>-5</v>
+      </c>
+      <c r="H14" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="56"/>
+    </row>
+    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" s="6">
         <v>3</v>
@@ -3751,12 +3774,12 @@
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="32"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="7" t="s">
         <v>17</v>
       </c>
@@ -3772,18 +3795,18 @@
       <c r="G16" s="6">
         <v>0</v>
       </c>
-      <c r="H16" s="55" t="s">
-        <v>56</v>
+      <c r="H16" s="22" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="32"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="7">
         <v>3</v>
@@ -3795,13 +3818,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H17" s="55" t="s">
-        <v>57</v>
+      <c r="H17" s="22" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="32"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="6" t="s">
         <v>19</v>
       </c>
@@ -3819,17 +3842,17 @@
         <v>2</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
-      <c r="B19" s="32"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19" s="7">
         <v>1</v>
@@ -3842,12 +3865,12 @@
         <v>0.5</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
-      <c r="B20" s="32"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="7" t="s">
         <v>22</v>
       </c>
@@ -3864,13 +3887,13 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
-      <c r="B21" s="32"/>
+      <c r="A21" s="28"/>
+      <c r="B21" s="28"/>
       <c r="C21" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" s="7">
         <v>3</v>
@@ -3882,8 +3905,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
-      <c r="B22" s="32"/>
+      <c r="A22" s="28"/>
+      <c r="B22" s="28"/>
       <c r="C22" s="7" t="s">
         <v>29</v>
       </c>
@@ -3900,13 +3923,13 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
-      <c r="B23" s="32"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="28"/>
       <c r="C23" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E23" s="7">
         <v>1</v>
@@ -3918,13 +3941,13 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
       <c r="C24" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E24" s="7">
         <v>2</v>
@@ -4255,6 +4278,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A3:A24"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B10:B24"/>
+    <mergeCell ref="E10:E12"/>
     <mergeCell ref="H7:H9"/>
     <mergeCell ref="H10:H12"/>
     <mergeCell ref="D2:G2"/>
@@ -4264,15 +4296,6 @@
     <mergeCell ref="F10:F12"/>
     <mergeCell ref="D6:G6"/>
     <mergeCell ref="G10:G12"/>
-    <mergeCell ref="A3:A24"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="B10:B24"/>
-    <mergeCell ref="E10:E12"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Author : Bhaskar Mamgai File modified : BhaskarMamgai.xlsx Description : TasksBreakDown/Sprint 2/Day 3 Story id : SSDMS_12345
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/BhaskarMamgai.xlsx
+++ b/TeamDetails/TasksBreakDown/BhaskarMamgai.xlsx
@@ -9,14 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Name 1" sheetId="1" r:id="rId1"/>
     <sheet name="Name 2" sheetId="2" r:id="rId2"/>
     <sheet name="Name 3" sheetId="4" r:id="rId3"/>
-    <sheet name="Name 4" sheetId="5" r:id="rId4"/>
-    <sheet name="Name 5" sheetId="6" r:id="rId5"/>
+    <sheet name="Name 5" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="61">
   <si>
     <t>Story ID</t>
   </si>
@@ -331,15 +330,6 @@
     <t>Make login button functionaL</t>
   </si>
   <si>
-    <t>Technical understanding</t>
-  </si>
-  <si>
-    <t>ng route</t>
-  </si>
-  <si>
-    <t>http.post</t>
-  </si>
-  <si>
     <t>Getting a response from backend database server (http.post())</t>
   </si>
   <si>
@@ -356,6 +346,25 @@
   </si>
   <si>
     <t>Perform/check client side validations are as per acceptance criteria.</t>
+  </si>
+  <si>
+    <t>Technical Understanding</t>
+  </si>
+  <si>
+    <t>Perform/check client side validations are as per acceptance criteria</t>
+  </si>
+  <si>
+    <t>In Dev</t>
+  </si>
+  <si>
+    <t>Fetching the req values from database</t>
+  </si>
+  <si>
+    <t>Getting/Reading a response from backend database server (http.post())</t>
+  </si>
+  <si>
+    <t>LOGIN 
+PAGE</t>
   </si>
 </sst>
 </file>
@@ -595,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -657,18 +666,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -690,27 +720,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -720,9 +759,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -732,34 +768,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1045,7 +1058,7 @@
   <dimension ref="A2:G47"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E8" sqref="E8:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,7 +1095,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="25" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="6"/>
@@ -1102,7 +1115,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="6"/>
       <c r="C4" s="10" t="s">
         <v>8</v>
@@ -1120,81 +1133,81 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="35" t="s">
+      <c r="A5" s="26"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="23">
-        <v>2</v>
-      </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23">
+      <c r="E5" s="33">
+        <v>2</v>
+      </c>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
     </row>
     <row r="7" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26" t="s">
+      <c r="A8" s="26"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="32">
-        <v>3</v>
-      </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26">
+      <c r="E8" s="39">
+        <v>53</v>
+      </c>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="27"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="34"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="31"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="27"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7" t="s">
         <v>11</v>
@@ -1212,7 +1225,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7" t="s">
         <v>15</v>
@@ -1230,7 +1243,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7" t="s">
         <v>16</v>
@@ -1247,7 +1260,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7" t="s">
         <v>17</v>
@@ -1265,7 +1278,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7" t="s">
         <v>18</v>
@@ -1283,7 +1296,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7" t="s">
         <v>19</v>
@@ -1301,7 +1314,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7" t="s">
         <v>20</v>
@@ -1319,7 +1332,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7" t="s">
         <v>22</v>
@@ -1337,7 +1350,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7" t="s">
         <v>24</v>
@@ -1355,7 +1368,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7" t="s">
         <v>29</v>
@@ -1698,11 +1711,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A3:A20"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C10"/>
@@ -1711,6 +1719,11 @@
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="F5:F7"/>
+    <mergeCell ref="A3:A20"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2294,10 +2307,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G46"/>
+  <dimension ref="A2:H46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2310,7 +2323,7 @@
     <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -2332,197 +2345,365 @@
       <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="H2" s="57" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="28">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
       <c r="G3" s="2">
         <f>E3-F3</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="H3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G46" si="0">E4-F4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+        <f t="shared" ref="G4:G18" si="0">E4-F4</f>
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="H5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="35"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="H6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.5</v>
+      </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>6</v>
+      </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+        <v>-5</v>
+      </c>
+      <c r="H8" s="58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.5</v>
+      </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="H10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="35"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="H11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="2">
+        <v>4</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
       <c r="G12" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="H12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="35"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.5</v>
+      </c>
       <c r="G13" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="2">
+        <v>4</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
       <c r="G14" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="35"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="2">
+        <v>3</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
       <c r="G15" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
       <c r="G16" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
       <c r="G17" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="2">
+        <v>2</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
       <c r="G18" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2533,7 +2714,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G4:G46" si="1">E19-F19</f>
         <v>0</v>
       </c>
     </row>
@@ -2545,7 +2726,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2557,7 +2738,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2569,7 +2750,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2581,7 +2762,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2593,7 +2774,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2605,7 +2786,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2617,7 +2798,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2629,7 +2810,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2641,7 +2822,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2653,7 +2834,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2665,7 +2846,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2677,7 +2858,7 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2689,7 +2870,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2701,7 +2882,7 @@
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2713,7 +2894,7 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2725,7 +2906,7 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2737,7 +2918,7 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2749,7 +2930,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2761,7 +2942,7 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2773,7 +2954,7 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2785,7 +2966,7 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2797,7 +2978,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2809,7 +2990,7 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2821,7 +3002,7 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2833,7 +3014,7 @@
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2845,7 +3026,7 @@
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2857,11 +3038,15 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:A18"/>
+    <mergeCell ref="B3:B18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2869,647 +3054,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H46"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" customWidth="1"/>
-    <col min="5" max="5" width="67.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="2">
-        <v>2</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2">
-        <f>F3-G3</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2">
-        <f t="shared" ref="H4:H46" si="0">F4-G4</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D3:D5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="B10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3548,7 +3099,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3557,15 +3108,15 @@
       <c r="C2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="43"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="53"/>
     </row>
     <row r="3" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="41" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="6"/>
@@ -3582,24 +3133,24 @@
         <v>2</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="49"/>
+      <c r="A4" s="42"/>
       <c r="B4" s="6"/>
       <c r="C4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="53" t="s">
+      <c r="D4" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="55"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:9" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="11" t="s">
@@ -3614,107 +3165,107 @@
         <v>2</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="17"/>
       <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="47"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="56"/>
     </row>
     <row r="7" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="36" t="s">
+      <c r="A7" s="29"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="23">
-        <v>2</v>
-      </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H7" s="40" t="s">
-        <v>55</v>
+      <c r="E7" s="33">
+        <v>2</v>
+      </c>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H7" s="43" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="40"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="43"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="27"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="44"/>
-      <c r="D9" s="51"/>
+      <c r="D9" s="46"/>
       <c r="E9" s="44"/>
       <c r="F9" s="44"/>
       <c r="G9" s="44"/>
-      <c r="H9" s="40"/>
+      <c r="H9" s="43"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="26">
+      <c r="A10" s="35"/>
+      <c r="B10" s="28">
         <f>SUM(E10:E24)</f>
         <v>23.5</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="26">
-        <v>0</v>
-      </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26">
-        <v>0</v>
-      </c>
-      <c r="H10" s="40" t="s">
-        <v>55</v>
+      <c r="E10" s="28">
+        <v>0</v>
+      </c>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28">
+        <v>0</v>
+      </c>
+      <c r="H10" s="43" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="40"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="43"/>
     </row>
     <row r="12" spans="1:9" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="40"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="43"/>
     </row>
     <row r="13" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="6" t="s">
         <v>11</v>
       </c>
@@ -3731,17 +3282,17 @@
         <v>0.5</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
       <c r="C14" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E14" s="6">
         <v>1</v>
@@ -3752,14 +3303,14 @@
       <c r="G14" s="21">
         <v>-5</v>
       </c>
-      <c r="H14" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14" s="56"/>
+      <c r="H14" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14" s="23"/>
     </row>
     <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
+      <c r="A15" s="35"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="6" t="s">
         <v>16</v>
       </c>
@@ -3774,12 +3325,12 @@
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="7" t="s">
         <v>17</v>
       </c>
@@ -3796,12 +3347,12 @@
         <v>0</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="7" t="s">
         <v>18</v>
       </c>
@@ -3819,12 +3370,12 @@
         <v>2</v>
       </c>
       <c r="H17" s="22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="6" t="s">
         <v>19</v>
       </c>
@@ -3842,12 +3393,12 @@
         <v>2</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="7" t="s">
         <v>20</v>
       </c>
@@ -3865,12 +3416,12 @@
         <v>0.5</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
       <c r="C20" s="7" t="s">
         <v>22</v>
       </c>
@@ -3887,13 +3438,13 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="28"/>
-      <c r="B21" s="28"/>
+      <c r="A21" s="35"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E21" s="7">
         <v>3</v>
@@ -3905,8 +3456,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28"/>
+      <c r="A22" s="35"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="7" t="s">
         <v>29</v>
       </c>
@@ -3923,8 +3474,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="7" t="s">
         <v>47</v>
       </c>
@@ -3941,13 +3492,13 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
       <c r="C24" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E24" s="7">
         <v>2</v>
@@ -4278,6 +3829,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="G10:G12"/>
     <mergeCell ref="A3:A24"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="C7:C9"/>
@@ -4287,15 +3847,6 @@
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="B10:B24"/>
     <mergeCell ref="E10:E12"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="G10:G12"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Author : Bhaskar Mamgai File modified : BhaskarMamgai.xlsx Description : TasksBreakDown/Sprint 2/Day 4
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/BhaskarMamgai.xlsx
+++ b/TeamDetails/TasksBreakDown/BhaskarMamgai.xlsx
@@ -672,18 +672,46 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -696,29 +724,32 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -726,12 +757,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -749,31 +774,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1095,7 +1095,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="38" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="6"/>
@@ -1115,7 +1115,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="6"/>
       <c r="C4" s="10" t="s">
         <v>8</v>
@@ -1133,81 +1133,81 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="29" t="s">
+      <c r="A5" s="28"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="33">
-        <v>2</v>
-      </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33">
+      <c r="E5" s="27">
+        <v>2</v>
+      </c>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
     </row>
     <row r="7" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28" t="s">
+      <c r="A8" s="28"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="36">
         <v>53</v>
       </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28">
+      <c r="F8" s="30"/>
+      <c r="G8" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="34"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="31"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="38"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="35"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="34"/>
+      <c r="F10" s="31"/>
       <c r="G10" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7" t="s">
         <v>11</v>
@@ -1225,7 +1225,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7" t="s">
         <v>15</v>
@@ -1243,7 +1243,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7" t="s">
         <v>16</v>
@@ -1260,7 +1260,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7" t="s">
         <v>17</v>
@@ -1278,7 +1278,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7" t="s">
         <v>18</v>
@@ -1296,7 +1296,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7" t="s">
         <v>19</v>
@@ -1314,7 +1314,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7" t="s">
         <v>20</v>
@@ -1332,7 +1332,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7" t="s">
         <v>22</v>
@@ -1350,7 +1350,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7" t="s">
         <v>24</v>
@@ -1368,7 +1368,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7" t="s">
         <v>29</v>
@@ -1711,6 +1711,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A3:A20"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C10"/>
@@ -1719,11 +1724,6 @@
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="F5:F7"/>
-    <mergeCell ref="A3:A20"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2309,8 +2309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B18"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2345,16 +2345,16 @@
       <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="57" t="s">
+      <c r="H2" s="25" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="28">
-        <v>18</v>
+      <c r="B3" s="30">
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
@@ -2377,8 +2377,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2400,8 +2400,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2423,8 +2423,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2446,8 +2446,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
-      <c r="B7" s="35"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
@@ -2469,8 +2469,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
-      <c r="B8" s="35"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
@@ -2487,13 +2487,13 @@
         <f t="shared" si="0"/>
         <v>-5</v>
       </c>
-      <c r="H8" s="58" t="s">
-        <v>57</v>
+      <c r="H8" s="26" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
@@ -2515,8 +2515,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
@@ -2538,8 +2538,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
-      <c r="B11" s="35"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
@@ -2561,8 +2561,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="2" t="s">
         <v>19</v>
       </c>
@@ -2584,8 +2584,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="2" t="s">
         <v>20</v>
       </c>
@@ -2607,8 +2607,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
@@ -2619,16 +2619,16 @@
         <v>4</v>
       </c>
       <c r="F14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
       <c r="C15" s="2" t="s">
         <v>24</v>
       </c>
@@ -2647,8 +2647,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="2" t="s">
         <v>29</v>
       </c>
@@ -2667,8 +2667,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="2" t="s">
         <v>47</v>
       </c>
@@ -2687,8 +2687,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="2" t="s">
         <v>36</v>
       </c>
@@ -2714,7 +2714,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2">
-        <f t="shared" ref="G4:G46" si="1">E19-F19</f>
+        <f t="shared" ref="G4:G21" si="1">E19-F19</f>
         <v>0</v>
       </c>
     </row>
@@ -2750,7 +2750,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G19:G46" si="2">E22-F22</f>
         <v>0</v>
       </c>
     </row>
@@ -2762,7 +2762,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2774,7 +2774,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2786,7 +2786,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2798,7 +2798,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2810,7 +2810,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2822,7 +2822,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2834,7 +2834,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2846,7 +2846,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2858,7 +2858,7 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2870,7 +2870,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2894,7 +2894,7 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2906,7 +2906,7 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2918,7 +2918,7 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2930,7 +2930,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2942,7 +2942,7 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2954,7 +2954,7 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2966,7 +2966,7 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2978,7 +2978,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2990,7 +2990,7 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3002,7 +3002,7 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3014,7 +3014,7 @@
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3026,7 +3026,7 @@
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3038,7 +3038,7 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3108,15 +3108,15 @@
       <c r="C2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="53"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="47"/>
     </row>
     <row r="3" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="52" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="6"/>
@@ -3137,20 +3137,20 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
+      <c r="A4" s="53"/>
       <c r="B4" s="6"/>
       <c r="C4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="50"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="59"/>
     </row>
     <row r="5" spans="1:9" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="11" t="s">
@@ -3169,103 +3169,103 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="17"/>
       <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="56"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="51"/>
     </row>
     <row r="7" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="30" t="s">
+      <c r="A7" s="39"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="33">
-        <v>2</v>
-      </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H7" s="43" t="s">
+      <c r="E7" s="27">
+        <v>2</v>
+      </c>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H7" s="44" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="43"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="44"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="43"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="44"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
-      <c r="B10" s="28">
+      <c r="A10" s="32"/>
+      <c r="B10" s="30">
         <f>SUM(E10:E24)</f>
         <v>23.5</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="28">
-        <v>0</v>
-      </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28">
-        <v>0</v>
-      </c>
-      <c r="H10" s="43" t="s">
+      <c r="E10" s="30">
+        <v>0</v>
+      </c>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30">
+        <v>0</v>
+      </c>
+      <c r="H10" s="44" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="43"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="44"/>
     </row>
     <row r="12" spans="1:9" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="43"/>
+      <c r="A12" s="44"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="44"/>
     </row>
     <row r="13" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="6" t="s">
         <v>11</v>
       </c>
@@ -3286,8 +3286,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="6" t="s">
         <v>15</v>
       </c>
@@ -3309,8 +3309,8 @@
       <c r="I14" s="23"/>
     </row>
     <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
       <c r="C15" s="6" t="s">
         <v>16</v>
       </c>
@@ -3329,8 +3329,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="7" t="s">
         <v>17</v>
       </c>
@@ -3351,8 +3351,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="7" t="s">
         <v>18</v>
       </c>
@@ -3374,8 +3374,8 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="6" t="s">
         <v>19</v>
       </c>
@@ -3397,8 +3397,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
       <c r="C19" s="7" t="s">
         <v>20</v>
       </c>
@@ -3420,8 +3420,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="35"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
       <c r="C20" s="7" t="s">
         <v>22</v>
       </c>
@@ -3438,8 +3438,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
-      <c r="B21" s="35"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
       <c r="C21" s="7" t="s">
         <v>24</v>
       </c>
@@ -3456,8 +3456,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
-      <c r="B22" s="35"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
       <c r="C22" s="7" t="s">
         <v>29</v>
       </c>
@@ -3474,8 +3474,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
-      <c r="B23" s="35"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
       <c r="C23" s="7" t="s">
         <v>47</v>
       </c>
@@ -3492,8 +3492,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="34"/>
-      <c r="B24" s="34"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
       <c r="C24" s="7" t="s">
         <v>36</v>
       </c>
@@ -3829,6 +3829,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A3:A24"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B10:B24"/>
+    <mergeCell ref="E10:E12"/>
     <mergeCell ref="H7:H9"/>
     <mergeCell ref="H10:H12"/>
     <mergeCell ref="D2:G2"/>
@@ -3838,15 +3847,6 @@
     <mergeCell ref="F10:F12"/>
     <mergeCell ref="D6:G6"/>
     <mergeCell ref="G10:G12"/>
-    <mergeCell ref="A3:A24"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="B10:B24"/>
-    <mergeCell ref="E10:E12"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>